<commit_message>
New CNN architecture based on Keagle Compeititions Research, 99.52% accuracy, 99.515% F1 Score.
</commit_message>
<xml_diff>
--- a/Model Performance.xlsx
+++ b/Model Performance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cipri\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academia\Kings_College_London\Semester_2\Deep_Learning_&amp;_Neural_Networks\Coursework_I\MNIST_deeplearning_recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B495659-8B50-4B41-82D9-6C6794E40D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8718D087-AE8E-408A-81DA-C76FB3FA8A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="4995" windowWidth="37350" windowHeight="23835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19290" yWindow="4875" windowWidth="37350" windowHeight="23835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
   <si>
     <t>version</t>
   </si>
@@ -313,6 +313,18 @@
   </si>
   <si>
     <t>CNNs based on Papers - See Notes for network summary</t>
+  </si>
+  <si>
+    <t>99.69, 99.65, 99.90, 99.21, 99.29, 99.44, 99.27, 99.13, 99.90, 99.70</t>
+  </si>
+  <si>
+    <t>99.59, 99.74, 99.52, 99.80, 99.69, 99.10, 99.69, 99.61, 99.38, 99.01</t>
+  </si>
+  <si>
+    <t>99.64, 99.69, 99.71, 99.51, 99.49, 99.27, 99.48, 99.37, 99.64, 99.35</t>
+  </si>
+  <si>
+    <t>highest accuracy during training 99.60%</t>
   </si>
 </sst>
 </file>
@@ -807,46 +819,19 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -861,6 +846,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,7 +1157,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="B33" sqref="B33:O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1178,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="29" t="s">
         <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1213,26 +1225,26 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="21" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="23"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="33"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="7">
         <v>0.1</v>
       </c>
@@ -1275,7 +1287,7 @@
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="7">
         <v>0.2</v>
       </c>
@@ -1318,7 +1330,7 @@
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="7">
         <v>0.3</v>
       </c>
@@ -1361,7 +1373,7 @@
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="16">
         <v>0.4</v>
       </c>
@@ -1404,7 +1416,7 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="7">
         <v>0.5</v>
       </c>
@@ -1447,7 +1459,7 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="7">
         <v>0.6</v>
       </c>
@@ -1490,26 +1502,26 @@
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="26"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="25"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="7">
         <v>0.7</v>
       </c>
@@ -1519,22 +1531,22 @@
       <c r="D11" s="1">
         <v>4</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="29"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="36"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="7">
         <v>0.8</v>
       </c>
@@ -1544,22 +1556,22 @@
       <c r="D12" s="1">
         <v>8</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="29"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="36"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="16">
         <v>0.9</v>
       </c>
@@ -1584,7 +1596,7 @@
       <c r="I13" s="18">
         <v>99.255256000000003</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="22">
         <v>2.4725999999999998E-6</v>
       </c>
       <c r="K13" s="18">
@@ -1604,7 +1616,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="7">
         <v>1</v>
       </c>
@@ -1649,7 +1661,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -1692,7 +1704,7 @@
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="7">
         <v>1.2</v>
       </c>
@@ -1737,7 +1749,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="7">
         <v>1.3</v>
       </c>
@@ -1777,12 +1789,12 @@
       <c r="N17" s="10">
         <v>99.106214874168799</v>
       </c>
-      <c r="O17" s="30" t="s">
+      <c r="O17" s="37" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="7">
         <v>1.4</v>
       </c>
@@ -1822,10 +1834,10 @@
       <c r="N18" s="10">
         <v>98.898370638204597</v>
       </c>
-      <c r="O18" s="31"/>
+      <c r="O18" s="38"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="7">
         <v>1.5</v>
       </c>
@@ -1865,29 +1877,29 @@
       <c r="N19" s="10">
         <v>98.940286378191104</v>
       </c>
-      <c r="O19" s="32"/>
+      <c r="O19" s="39"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="26"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="25"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="7">
         <v>1.6</v>
       </c>
@@ -1932,7 +1944,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="7">
         <v>1.7</v>
       </c>
@@ -1957,7 +1969,7 @@
       <c r="I22" s="1">
         <v>98.966266000000005</v>
       </c>
-      <c r="J22" s="33">
+      <c r="J22" s="21">
         <v>7.5234000000000005E-5</v>
       </c>
       <c r="K22" s="1">
@@ -1977,7 +1989,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="7">
         <v>1.8</v>
       </c>
@@ -2022,7 +2034,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="7">
         <v>1.9</v>
       </c>
@@ -2065,7 +2077,7 @@
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="39"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="7">
         <v>2</v>
       </c>
@@ -2108,7 +2120,7 @@
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="7">
         <v>2.1</v>
       </c>
@@ -2151,7 +2163,7 @@
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="39"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="7">
         <v>2.2000000000000002</v>
       </c>
@@ -2194,26 +2206,26 @@
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="39"/>
-      <c r="B28" s="24" t="s">
+      <c r="A28" s="30"/>
+      <c r="B28" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="26"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="25"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="39"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -2258,7 +2270,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="16">
         <v>2.4</v>
       </c>
@@ -2283,7 +2295,7 @@
       <c r="I30" s="18">
         <v>99.344182000000004</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="22">
         <v>3.2853999999999999E-6</v>
       </c>
       <c r="K30" s="18">
@@ -2301,66 +2313,92 @@
       <c r="O30" s="2"/>
     </row>
     <row r="31" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="26"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="25"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="7">
         <v>2.5</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="2"/>
+      <c r="C32" s="1">
+        <v>40</v>
+      </c>
+      <c r="D32" s="1">
+        <v>16</v>
+      </c>
+      <c r="E32" s="1">
+        <v>99.52</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I32" s="10">
+        <v>99.466457000000005</v>
+      </c>
+      <c r="J32" s="1">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="K32" s="10">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="L32" s="1">
+        <v>99.518290561269794</v>
+      </c>
+      <c r="M32" s="1">
+        <v>99.513328949604002</v>
+      </c>
+      <c r="N32" s="10">
+        <v>99.515323065414805</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
-      <c r="B33" s="24" t="s">
+      <c r="A33" s="27"/>
+      <c r="B33" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="26"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="25"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="7">
         <v>2.6</v>
       </c>
@@ -2379,7 +2417,7 @@
       <c r="O34" s="2"/>
     </row>
     <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="7"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2396,7 +2434,7 @@
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="7"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2413,7 +2451,7 @@
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="7"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2430,7 +2468,7 @@
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="7"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2447,7 +2485,7 @@
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="7"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2464,7 +2502,7 @@
       <c r="O39" s="2"/>
     </row>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="36"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="7"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2481,7 +2519,7 @@
       <c r="O40" s="2"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="36"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="7"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2498,7 +2536,7 @@
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="7"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2515,7 +2553,7 @@
       <c r="O42" s="2"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="36"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="7"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2532,7 +2570,7 @@
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="36"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="7"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2549,7 +2587,7 @@
       <c r="O44" s="2"/>
     </row>
     <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="36"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="7"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2566,7 +2604,7 @@
       <c r="O45" s="2"/>
     </row>
     <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="36"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="7"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2583,7 +2621,7 @@
       <c r="O46" s="2"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="36"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="7"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2600,7 +2638,7 @@
       <c r="O47" s="2"/>
     </row>
     <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="36"/>
+      <c r="A48" s="27"/>
       <c r="B48" s="7"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2617,7 +2655,7 @@
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="37"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="8"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>

</xml_diff>

<commit_message>
Added folder containing best trained models. Updated model performance excel file. Added data augmentation. Fully implemented session closure/resource release after training ends.
</commit_message>
<xml_diff>
--- a/Model Performance.xlsx
+++ b/Model Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academia\Kings_College_London\Semester_2\Deep_Learning_&amp;_Neural_Networks\Coursework_I\MNIST_deeplearning_recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8718D087-AE8E-408A-81DA-C76FB3FA8A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9D439D-2C67-4202-A8A0-1992380D0E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19290" yWindow="4875" windowWidth="37350" windowHeight="23835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21375" yWindow="6825" windowWidth="38925" windowHeight="21975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
   <si>
     <t>version</t>
   </si>
@@ -309,9 +309,6 @@
     <t>NEW CNN ARCHITECTURE - BASED ON KAGGLE CNN MNIST COMPETITIONS (with custom optimisations) - https://www.kaggle.com/code/cdeotte/how-to-choose-cnn-architecture-mnist</t>
   </si>
   <si>
-    <t>NEW CNN ARCHITECTURE - BASED ON RESEARCH PAPER: "AN ENSEMBLE OF SIMPLE CONVOLUTIONAL NEURAL NETWORK MODELS FOR MNIST DIGIT RECOGNITION" - AVAILABLE AT: https://paperswithcode.com/paper/an-ensemble-of-simple-convolutional-neural</t>
-  </si>
-  <si>
     <t>CNNs based on Papers - See Notes for network summary</t>
   </si>
   <si>
@@ -325,6 +322,96 @@
   </si>
   <si>
     <t>highest accuracy during training 99.60%</t>
+  </si>
+  <si>
+    <t>PREVIOUS CNN ARCHITECTURE WITH ADDED DATA AUGMENTATION ON THE TRAINING SET</t>
+  </si>
+  <si>
+    <t>99.90, 99.56, 99.61, 99.70, 99.19, 99.55, 99.48, 99.61, 99.69, 99.60</t>
+  </si>
+  <si>
+    <t>100.00, 99.82, 99.81, 99.70, 99.69, 99.55, 99.06, 99.42, 99.59, 99.21</t>
+  </si>
+  <si>
+    <t>99.95, 99.69, 99.71, 99.70, 99.44, 99.55, 99.27, 99.51, 99.64, 99.40</t>
+  </si>
+  <si>
+    <t>highest accuracy during training 99.72%</t>
+  </si>
+  <si>
+    <t>99.90, 99.65, 99.71, 99.60, 99.59, 99.78, 99.38, 99.71, 99.69, 99.70</t>
+  </si>
+  <si>
+    <t>99.69, 100.00, 99.81, 99.80, 99.49, 99.55, 99.69, 99.71, 99.59, 99.31</t>
+  </si>
+  <si>
+    <t>99.80, 99.82, 99.76, 99.70, 99.54, 99.66, 99.53, 99.71, 99.64, 99.50</t>
+  </si>
+  <si>
+    <t>99.69, 99.65, 99.42, 99.31, 99.39, 99.55, 99.79, 99.71, 99.69, 99.11</t>
+  </si>
+  <si>
+    <t>100.00, 99.74, 99.61, 99.80, 98.98, 99.55, 99.06, 99.61, 99.49, 99.41</t>
+  </si>
+  <si>
+    <t>99.85, 99.69, 99.52, 99.56, 99.18, 99.55, 99.42, 99.66, 99.59, 99.26</t>
+  </si>
+  <si>
+    <t>99.80, 99.91, 99.42, 99.21, 99.49, 99.66, 99.37, 99.51, 99.79, 99.90</t>
+  </si>
+  <si>
+    <t>99.90, 99.38, 99.71, 99.90, 99.90, 99.55, 99.37, 99.51, 99.59, 99.31</t>
+  </si>
+  <si>
+    <t>99.85, 99.65, 99.56, 99.56, 99.70, 99.61, 99.37, 99.51, 99.69, 99.60</t>
+  </si>
+  <si>
+    <t>PREVIOUS CNN ARCHITECTURE WITH  DOUBLE THE NEURONS FOR ALL LAYERS</t>
+  </si>
+  <si>
+    <t>99.80, 99.65, 99.61, 99.70, 99.39, 99.55, 99.79, 99.61, 99.90, 99.80</t>
+  </si>
+  <si>
+    <t>99.90, 99.82, 99.90, 99.80, 99.80, 99.66, 99.48, 99.51, 99.49, 99.41</t>
+  </si>
+  <si>
+    <t>99.85, 99.74, 99.76, 99.75, 99.59, 99.61, 99.63, 99.56, 99.69, 99.60</t>
+  </si>
+  <si>
+    <t>99.80, 99.82, 99.90, 99.60, 99.29, 99.78, 99.69, 99.13, 99.69, 99.70</t>
+  </si>
+  <si>
+    <t>100.00, 99.56, 99.22, 99.80, 99.69, 99.78, 99.69, 99.81, 99.59, 99.31</t>
+  </si>
+  <si>
+    <t>99.90, 99.69, 99.56, 99.70, 99.49, 99.78, 99.69, 99.47, 99.64, 99.50</t>
+  </si>
+  <si>
+    <t>99.69, 99.74, 99.42, 99.70, 99.90, 99.66, 99.79, 99.51, 99.90, 99.21</t>
+  </si>
+  <si>
+    <t>100.00, 99.65, 99.42, 99.80, 99.19, 99.78, 99.90, 99.51, 99.59, 99.70</t>
+  </si>
+  <si>
+    <t>99.85, 99.69, 99.42, 99.75, 99.54, 99.72, 99.84, 99.51, 99.74, 99.46</t>
+  </si>
+  <si>
+    <t>99.39, 99.65, 99.81, 98.92, 99.59, 99.77, 99.68, 99.71, 99.90, 99.21</t>
+  </si>
+  <si>
+    <t>100.00, 99.82, 99.61, 100.00, 99.39, 98.99, 99.06, 99.32, 99.79, 99.50</t>
+  </si>
+  <si>
+    <t>99.69, 99.74, 99.71, 99.46, 99.49, 99.38, 99.37, 99.51, 99.85, 99.36</t>
+  </si>
+  <si>
+    <t>99.59, 99.38, 99.80, 99.12, 98.79, 99.77, 99.37, 98.46, 99.59, 99.80</t>
+  </si>
+  <si>
+    <t>99.69, 99.56, 98.55, 99.90, 99.80, 98.99, 99.37, 99.71, 99.69, 98.32</t>
+  </si>
+  <si>
+    <t>99.64, 99.47, 99.17, 99.51, 99.29, 99.38, 99.37, 99.08, 99.64, 99.05</t>
   </si>
 </sst>
 </file>
@@ -356,7 +443,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +486,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -763,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -872,6 +965,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1157,7 +1259,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:O33"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2416,7 @@
     </row>
     <row r="31" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="23" t="s">
         <v>93</v>
@@ -2348,13 +2450,13 @@
         <v>99.52</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="I32" s="10">
         <v>99.466457000000005</v>
@@ -2375,13 +2477,13 @@
         <v>99.515323065414805</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
       <c r="B33" s="23" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
@@ -2402,178 +2504,418 @@
       <c r="B34" s="7">
         <v>2.6</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="2"/>
+      <c r="C34" s="1">
+        <v>40</v>
+      </c>
+      <c r="D34" s="1">
+        <v>16</v>
+      </c>
+      <c r="E34" s="1">
+        <v>99.59</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I34" s="10">
+        <v>99.544264999999996</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="K34" s="10">
+        <v>1.21E-2</v>
+      </c>
+      <c r="L34" s="1">
+        <v>99.589554423595303</v>
+      </c>
+      <c r="M34" s="1">
+        <v>99.585237428860296</v>
+      </c>
+      <c r="N34" s="10">
+        <v>99.587207772325797</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="10"/>
+      <c r="B35" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="C35" s="1">
+        <v>35</v>
+      </c>
+      <c r="D35" s="1">
+        <v>16</v>
+      </c>
+      <c r="E35" s="1">
+        <v>99.62</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I35" s="10">
+        <v>99.566501000000002</v>
+      </c>
+      <c r="J35" s="1">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="K35" s="10">
+        <v>1.18E-2</v>
+      </c>
+      <c r="L35" s="1">
+        <v>99.607926689515807</v>
+      </c>
+      <c r="M35" s="1">
+        <v>99.612412809604606</v>
+      </c>
+      <c r="N35" s="10">
+        <v>99.6098140371314</v>
+      </c>
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="10"/>
+      <c r="B36" s="40">
+        <v>2.8</v>
+      </c>
+      <c r="C36" s="41">
+        <v>30</v>
+      </c>
+      <c r="D36" s="41">
+        <v>16</v>
+      </c>
+      <c r="E36" s="41">
+        <v>99.68</v>
+      </c>
+      <c r="F36" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="I36" s="42">
+        <v>99.644305000000003</v>
+      </c>
+      <c r="J36" s="41">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="K36" s="42">
+        <v>1.11E-2</v>
+      </c>
+      <c r="L36" s="41">
+        <v>99.680366069887796</v>
+      </c>
+      <c r="M36" s="41">
+        <v>99.677054266530206</v>
+      </c>
+      <c r="N36" s="42">
+        <v>99.678523759825197</v>
+      </c>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="10"/>
+      <c r="B37" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="C37" s="1">
+        <v>50</v>
+      </c>
+      <c r="D37" s="1">
+        <v>16</v>
+      </c>
+      <c r="E37" s="1">
+        <v>99.64</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I37" s="10">
+        <v>99.599846999999997</v>
+      </c>
+      <c r="J37" s="1">
+        <v>2.06E-2</v>
+      </c>
+      <c r="K37" s="10">
+        <v>1.24E-2</v>
+      </c>
+      <c r="L37" s="1">
+        <v>99.6403133430005</v>
+      </c>
+      <c r="M37" s="1">
+        <v>99.644440479456193</v>
+      </c>
+      <c r="N37" s="10">
+        <v>99.642026518247505</v>
+      </c>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="10"/>
+      <c r="B38" s="7">
+        <v>3</v>
+      </c>
+      <c r="C38" s="1">
+        <v>80</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>99.65</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" s="10">
+        <v>99.610960000000006</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="K38" s="10">
+        <v>1.21E-2</v>
+      </c>
+      <c r="L38" s="1">
+        <v>99.652674678769301</v>
+      </c>
+      <c r="M38" s="1">
+        <v>99.653051558604702</v>
+      </c>
+      <c r="N38" s="10">
+        <v>99.652617732738705</v>
+      </c>
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="2"/>
+      <c r="B39" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="25"/>
     </row>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="27"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="10"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="41">
+        <v>35</v>
+      </c>
+      <c r="D40" s="41">
+        <v>16</v>
+      </c>
+      <c r="E40" s="41">
+        <v>99.67</v>
+      </c>
+      <c r="F40" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="H40" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" s="42">
+        <v>99.633188000000004</v>
+      </c>
+      <c r="J40" s="41">
+        <v>0.02</v>
+      </c>
+      <c r="K40" s="42">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L40" s="41">
+        <v>99.670541512184599</v>
+      </c>
+      <c r="M40" s="41">
+        <v>99.663504882977307</v>
+      </c>
+      <c r="N40" s="42">
+        <v>99.666888463563495</v>
+      </c>
       <c r="O40" s="2"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="10"/>
+      <c r="B41" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>45</v>
+      </c>
+      <c r="D41" s="1">
+        <v>16</v>
+      </c>
+      <c r="E41" s="1">
+        <v>99.53</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" s="10">
+        <v>99.477570999999998</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1.67E-2</v>
+      </c>
+      <c r="K41" s="10">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="L41" s="1">
+        <v>99.531045780225796</v>
+      </c>
+      <c r="M41" s="1">
+        <v>99.5246748236044</v>
+      </c>
+      <c r="N41" s="10">
+        <v>99.527555282444695</v>
+      </c>
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="10"/>
+      <c r="B42" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="C42" s="1">
+        <v>40</v>
+      </c>
+      <c r="D42" s="1">
+        <v>16</v>
+      </c>
+      <c r="E42" s="1">
+        <v>99.56</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I42" s="10">
+        <v>99.510914</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="K42" s="10">
+        <v>1.67E-2</v>
+      </c>
+      <c r="L42" s="1">
+        <v>99.563259233698503</v>
+      </c>
+      <c r="M42" s="1">
+        <v>99.549495507139298</v>
+      </c>
+      <c r="N42" s="10">
+        <v>99.555650691517997</v>
+      </c>
       <c r="O42" s="2"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="10"/>
+      <c r="B43" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="C43" s="1">
+        <v>30</v>
+      </c>
+      <c r="D43" s="1">
+        <v>16</v>
+      </c>
+      <c r="E43" s="1">
+        <v>99.36</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I43" s="10">
+        <v>99.288606000000001</v>
+      </c>
+      <c r="J43" s="1">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="K43" s="10">
+        <v>1.72E-2</v>
+      </c>
+      <c r="L43" s="1">
+        <v>99.368582202754993</v>
+      </c>
+      <c r="M43" s="1">
+        <v>99.357723776517901</v>
+      </c>
+      <c r="N43" s="10">
+        <v>99.361231044924807</v>
+      </c>
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="B44" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="C44" s="1">
+        <v>50</v>
+      </c>
+      <c r="D44" s="1">
+        <v>16</v>
+      </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -2588,9 +2930,15 @@
     </row>
     <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="27"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="B45" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="C45" s="1">
+        <v>50</v>
+      </c>
+      <c r="D45" s="1">
+        <v>32</v>
+      </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -2673,7 +3021,7 @@
     </row>
     <row r="50" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="B33:O33"/>
     <mergeCell ref="A31:A49"/>
     <mergeCell ref="B28:O28"/>
@@ -2685,6 +3033,7 @@
     <mergeCell ref="E11:O11"/>
     <mergeCell ref="B20:O20"/>
     <mergeCell ref="O17:O19"/>
+    <mergeCell ref="B39:O39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added multiple trained models. Added code to create ensemble model, added code to test models in standalone mode. Updated EXCEL sheet with versions and metrics.
</commit_message>
<xml_diff>
--- a/Model Performance.xlsx
+++ b/Model Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academia\Kings_College_London\Semester_2\Deep_Learning_&amp;_Neural_Networks\Coursework_I\MNIST_deeplearning_recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9D439D-2C67-4202-A8A0-1992380D0E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD457CF2-C990-491F-A0A4-DFDA5A6D584E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21375" yWindow="6825" windowWidth="38925" windowHeight="21975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24255" yWindow="1395" windowWidth="27975" windowHeight="29970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="164">
   <si>
     <t>version</t>
   </si>
@@ -243,9 +243,6 @@
     <t>99.34, 99.60, 99.08, 99.01, 99.09, 98.43, 99.00, 99.22, 98.82, 98.95</t>
   </si>
   <si>
-    <t>Conv 32 - Pooling 2,2 - Conv 64 - Conv 64 - Pooling 2,2 - Flatten - Dense 100 - Dense 10</t>
-  </si>
-  <si>
     <t>BEST BATCH SIZE AND EPOCHS FROM LAST TRIALS</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
     <t>NEW CNN ARCHITECTURE - BASED ON KAGGLE CNN MNIST COMPETITIONS (with custom optimisations) - https://www.kaggle.com/code/cdeotte/how-to-choose-cnn-architecture-mnist</t>
   </si>
   <si>
-    <t>CNNs based on Papers - See Notes for network summary</t>
-  </si>
-  <si>
     <t>99.69, 99.65, 99.90, 99.21, 99.29, 99.44, 99.27, 99.13, 99.90, 99.70</t>
   </si>
   <si>
@@ -412,6 +406,117 @@
   </si>
   <si>
     <t>99.64, 99.47, 99.17, 99.51, 99.29, 99.38, 99.37, 99.08, 99.64, 99.05</t>
+  </si>
+  <si>
+    <t>PREVIOUS CNN ARCHITECTURE WITH  DOUBLE THE BATCH SIZE</t>
+  </si>
+  <si>
+    <t>99.59, 99.65, 99.71, 99.21, 99.80, 99.78, 99.58, 99.90, 99.59, 99.21</t>
+  </si>
+  <si>
+    <t>99.80, 99.82, 99.90, 100.00, 99.29, 99.44, 99.37, 99.42, 99.49, 99.41</t>
+  </si>
+  <si>
+    <t>99.69, 99.74, 99.81, 99.61, 99.54, 99.61, 99.48, 99.66, 99.54, 99.31</t>
+  </si>
+  <si>
+    <t>99.73% highest accuracy at epoch 42</t>
+  </si>
+  <si>
+    <t>99.90, 99.82, 99.90, 99.41, 99.39, 99.78, 99.27, 99.42, 99.49, 99.50</t>
+  </si>
+  <si>
+    <t>99.39, 99.47, 99.71, 99.80, 99.59, 99.55, 99.58, 99.71, 99.69, 99.41</t>
+  </si>
+  <si>
+    <t>99.64, 99.65, 99.81, 99.60, 99.49, 99.66, 99.43, 99.56, 99.59, 99.45</t>
+  </si>
+  <si>
+    <t>99.80, 99.47, 99.90, 99.70, 99.69, 99.33, 99.79, 99.03, 99.69, 99.70</t>
+  </si>
+  <si>
+    <t>100.00, 99.74, 99.22, 99.90, 99.49, 99.66, 99.06, 99.81, 99.69, 99.50</t>
+  </si>
+  <si>
+    <t>99.90, 99.60, 99.56, 99.80, 99.59, 99.50, 99.42, 99.42, 99.69, 99.60</t>
+  </si>
+  <si>
+    <t>ENSEMBLE CNN MODELS</t>
+  </si>
+  <si>
+    <t>99.9, 99.56, 99.9, 98.82, 99.29, 99.55, 99.37, 99.22, 99.49, 99.8</t>
+  </si>
+  <si>
+    <t>99.21, 99.91, 99.22, 99.8, 99.9, 99.22, 99.16, 99.51, 99.79, 99.01</t>
+  </si>
+  <si>
+    <t>99.59, 99.74, 99.56, 99.31, 99.59, 99.38, 99.27, 99.37, 99.64, 99.40</t>
+  </si>
+  <si>
+    <t>99.80, 99.74, 99.71, 99.41, 99.59, 99.33, 99.69, 99.42, 99.79, 99.80</t>
+  </si>
+  <si>
+    <t>99.80, 99.74, 99.81, 99.90, 99.80, 99.33, 99.58, 99.71, 99.69, 98.91</t>
+  </si>
+  <si>
+    <t>99.80, 99.74, 99.76, 99.65, 99.69, 99.33, 99.63, 99.56, 99.74, 99.35</t>
+  </si>
+  <si>
+    <t>99.80, 99.78, 99.52, 99.61, 99.29, 99.49, 99.48, 99.51, 99.49, 99.21</t>
+  </si>
+  <si>
+    <t>99.90, 100.00, 99.52, 100.00, 99.08, 99.33, 99.06, 99.61, 99.59, 99.01</t>
+  </si>
+  <si>
+    <t>99.69, 99.56, 99.52, 99.21, 99.49, 99.66, 99.89, 99.42, 99.39, 99.40</t>
+  </si>
+  <si>
+    <t>99.69, 99.56, 99.81, 99.51, 99.59, 99.33, 99.79, 99.80, 99.59, 98.82</t>
+  </si>
+  <si>
+    <t>100.00, 99.65, 99.71, 99.90, 98.68, 99.78, 99.27, 99.42, 99.69, 99.41</t>
+  </si>
+  <si>
+    <t>99.85, 99.60, 99.76, 99.70, 99.13, 99.55, 99.53, 99.61, 99.64, 99.11</t>
+  </si>
+  <si>
+    <t>dropout increased to 0.5</t>
+  </si>
+  <si>
+    <t>C32-BN-C32-BN-C32-BN-DO0.4-C64-BN-C64-BN-C64-BN-D00.4-F-D128-BN-DO0.4-D10</t>
+  </si>
+  <si>
+    <t>C32 - Pooling 2,2 - C64 - C64 - Pooling 2,2 - F - D100 - D10</t>
+  </si>
+  <si>
+    <t>99.80, 99.56, 99.90, 99.11, 99.49, 99.77, 99.58, 99.32, 99.90, 99.50</t>
+  </si>
+  <si>
+    <t>99.90, 99.74, 99.52, 99.70, 99.59, 99.10, 99.79, 99.42, 99.69, 99.41</t>
+  </si>
+  <si>
+    <t>99.85, 99.65, 99.71, 99.41, 99.54, 99.44, 99.69, 99.37, 99.79, 99.45</t>
+  </si>
+  <si>
+    <t>99.80, 99.91, 99.42, 98.73, 99.39, 99.89, 99.58, 99.42, 99.79, 99.60</t>
+  </si>
+  <si>
+    <t>99.69, 99.47, 99.42, 100.00, 99.59, 99.33, 99.69, 99.61, 99.49, 99.21</t>
+  </si>
+  <si>
+    <t>99.74, 99.69, 99.42, 99.36, 99.49, 99.61, 99.63, 99.51, 99.64, 99.40</t>
+  </si>
+  <si>
+    <t>99.69, 99.74, 99.98, 99.82, 99.49, 99.55, 99.69, 99.32, 99.79, 99.11</t>
+  </si>
+  <si>
+    <t>99.80, 99.74, 99.22, 99.98, 99.19, 99.22, 99.27, 99.81, 99.59, 99.50</t>
+  </si>
+  <si>
+    <t>99.75, 99.74, 99.56, 99.46, 99.34, 99.38, 99.48, 99.56, 99.69, 99.31</t>
+  </si>
+  <si>
+    <t> 99.477571</t>
   </si>
 </sst>
 </file>
@@ -493,7 +598,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -607,16 +712,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
+      <right/>
+      <top style="thick">
         <color auto="1"/>
       </top>
-      <bottom style="thick">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -625,67 +728,11 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thick">
         <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -805,43 +852,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thick">
         <color auto="1"/>
@@ -856,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -864,7 +874,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -877,24 +886,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -903,7 +901,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -916,65 +914,62 @@
     <xf numFmtId="11" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1256,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="E61" sqref="D61:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,7 +1264,7 @@
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="57.28515625" customWidth="1"/>
-    <col min="7" max="7" width="57.140625" customWidth="1"/>
+    <col min="7" max="7" width="57.7109375" customWidth="1"/>
     <col min="8" max="8" width="56.7109375" customWidth="1"/>
     <col min="9" max="9" width="12.140625" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
@@ -1280,74 +1275,74 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="33"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="7">
+      <c r="A4" s="24"/>
+      <c r="B4" s="6">
         <v>0.1</v>
       </c>
       <c r="C4" s="1">
@@ -1368,13 +1363,13 @@
       <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <v>98.932911000000004</v>
       </c>
       <c r="J4" s="1">
         <v>1.4E-3</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="8">
         <v>3.3799999999999997E-2</v>
       </c>
       <c r="L4" s="1">
@@ -1383,14 +1378,14 @@
       <c r="M4" s="1">
         <v>99.028999999999996</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="8">
         <v>99.033000000000001</v>
       </c>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
-      <c r="B5" s="7">
+      <c r="A5" s="24"/>
+      <c r="B5" s="6">
         <v>0.2</v>
       </c>
       <c r="C5" s="1">
@@ -1411,13 +1406,13 @@
       <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>99.010712999999996</v>
       </c>
       <c r="J5" s="1">
         <v>1.4E-3</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="8">
         <v>3.3799999999999997E-2</v>
       </c>
       <c r="L5" s="1">
@@ -1426,14 +1421,14 @@
       <c r="M5" s="1">
         <v>99.094999999999999</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="8">
         <v>99.1</v>
       </c>
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
-      <c r="B6" s="7">
+      <c r="A6" s="24"/>
+      <c r="B6" s="6">
         <v>0.3</v>
       </c>
       <c r="C6" s="1">
@@ -1454,13 +1449,13 @@
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>99.055184999999994</v>
       </c>
       <c r="J6" s="1">
         <v>5.7255000000000001E-4</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="8">
         <v>3.7600000000000001E-2</v>
       </c>
       <c r="L6" s="1">
@@ -1469,57 +1464,57 @@
       <c r="M6" s="1">
         <v>99.135000000000005</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="8">
         <v>99.137</v>
       </c>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
-      <c r="B7" s="16">
+      <c r="A7" s="24"/>
+      <c r="B7" s="10">
         <v>0.4</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="11">
         <v>50</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="11">
         <v>256</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="11">
         <v>99.16</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="12">
         <v>99.066294999999997</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="11">
         <v>2.7980000000000002E-4</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="12">
         <v>4.1300000000000003E-2</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="11">
         <v>99.161000000000001</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="11">
         <v>99.152000000000001</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="12">
         <v>99.156000000000006</v>
       </c>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30"/>
-      <c r="B8" s="7">
+      <c r="A8" s="24"/>
+      <c r="B8" s="6">
         <v>0.5</v>
       </c>
       <c r="C8" s="1">
@@ -1540,13 +1535,13 @@
       <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="8">
         <v>98.988491999999994</v>
       </c>
       <c r="J8" s="1">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="8">
         <v>5.2699999999999997E-2</v>
       </c>
       <c r="L8" s="1">
@@ -1555,14 +1550,14 @@
       <c r="M8" s="1">
         <v>99.08</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="8">
         <v>99.08</v>
       </c>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
-      <c r="B9" s="7">
+      <c r="A9" s="24"/>
+      <c r="B9" s="6">
         <v>0.6</v>
       </c>
       <c r="C9" s="1">
@@ -1583,13 +1578,13 @@
       <c r="H9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="8">
         <v>98.944040999999999</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="9">
         <v>7.6758999999999996E-4</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="8">
         <v>3.4299999999999997E-2</v>
       </c>
       <c r="L9" s="1">
@@ -1598,33 +1593,33 @@
       <c r="M9" s="1">
         <v>99.034000000000006</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="8">
         <v>99.036000000000001</v>
       </c>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
-      <c r="B10" s="23" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="25"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="22"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
-      <c r="B11" s="7">
+      <c r="A11" s="24"/>
+      <c r="B11" s="6">
         <v>0.7</v>
       </c>
       <c r="C11" s="1">
@@ -1633,23 +1628,23 @@
       <c r="D11" s="1">
         <v>4</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="36"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="30"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
-      <c r="B12" s="7">
+      <c r="A12" s="24"/>
+      <c r="B12" s="6">
         <v>0.8</v>
       </c>
       <c r="C12" s="1">
@@ -1658,68 +1653,68 @@
       <c r="D12" s="1">
         <v>8</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="36"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="30"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
-      <c r="B13" s="16">
+      <c r="A13" s="24"/>
+      <c r="B13" s="10">
         <v>0.9</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="11">
         <v>50</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="11">
         <v>16</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="11">
         <v>99.33</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="12">
         <v>99.255256000000003</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="16">
         <v>2.4725999999999998E-6</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="12">
         <v>4.1500000000000002E-2</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="11">
         <v>99.326675177448607</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="11">
         <v>99.3164187591223</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="12">
         <v>99.321161756984793</v>
       </c>
-      <c r="O13" s="20" t="s">
+      <c r="O13" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
-      <c r="B14" s="7">
+      <c r="A14" s="24"/>
+      <c r="B14" s="6">
         <v>1</v>
       </c>
       <c r="C14" s="1">
@@ -1740,13 +1735,13 @@
       <c r="H14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="8">
         <v>99.233034000000004</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="9">
         <v>9.0815999999999996E-6</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="8">
         <v>4.36E-2</v>
       </c>
       <c r="L14" s="1">
@@ -1755,16 +1750,16 @@
       <c r="M14" s="1">
         <v>99.300336697322194</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="8">
         <v>99.300524091796404</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="7">
+      <c r="A15" s="24"/>
+      <c r="B15" s="6">
         <v>1.1000000000000001</v>
       </c>
       <c r="C15" s="1">
@@ -1785,13 +1780,13 @@
       <c r="H15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="8">
         <v>99.221909999999994</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="9">
         <v>2.0018E-5</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="8">
         <v>4.6699999999999998E-2</v>
       </c>
       <c r="L15" s="1">
@@ -1800,14 +1795,14 @@
       <c r="M15" s="1">
         <v>99.287139783089401</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="8">
         <v>99.292292657329696</v>
       </c>
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="7">
+      <c r="A16" s="24"/>
+      <c r="B16" s="6">
         <v>1.2</v>
       </c>
       <c r="C16" s="1">
@@ -1828,13 +1823,13 @@
       <c r="H16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="8">
         <v>99.132992999999999</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="9">
         <v>7.1874999999999999E-5</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="8">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="L16" s="1">
@@ -1843,16 +1838,16 @@
       <c r="M16" s="1">
         <v>99.210567499653393</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="8">
         <v>99.211743415228398</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="7">
+      <c r="A17" s="24"/>
+      <c r="B17" s="6">
         <v>1.3</v>
       </c>
       <c r="C17" s="1">
@@ -1873,13 +1868,13 @@
       <c r="H17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <v>99.021842000000007</v>
       </c>
       <c r="J17" s="1">
         <v>1.9E-3</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="8">
         <v>3.39E-2</v>
       </c>
       <c r="L17" s="1">
@@ -1888,16 +1883,16 @@
       <c r="M17" s="1">
         <v>99.106243503123096</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="8">
         <v>99.106214874168799</v>
       </c>
-      <c r="O17" s="37" t="s">
+      <c r="O17" s="31" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
-      <c r="B18" s="7">
+      <c r="A18" s="24"/>
+      <c r="B18" s="6">
         <v>1.4</v>
       </c>
       <c r="C18" s="1">
@@ -1918,13 +1913,13 @@
       <c r="H18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="8">
         <v>98.788408000000004</v>
       </c>
       <c r="J18" s="1">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="8">
         <v>3.3799999999999997E-2</v>
       </c>
       <c r="L18" s="1">
@@ -1933,14 +1928,14 @@
       <c r="M18" s="1">
         <v>98.894968220825504</v>
       </c>
-      <c r="N18" s="10">
+      <c r="N18" s="8">
         <v>98.898370638204597</v>
       </c>
-      <c r="O18" s="38"/>
+      <c r="O18" s="32"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30"/>
-      <c r="B19" s="7">
+      <c r="A19" s="24"/>
+      <c r="B19" s="6">
         <v>1.5</v>
       </c>
       <c r="C19" s="1">
@@ -1961,13 +1956,13 @@
       <c r="H19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="8">
         <v>98.832890000000006</v>
       </c>
       <c r="J19" s="1">
         <v>2.07E-2</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="8">
         <v>0.03</v>
       </c>
       <c r="L19" s="1">
@@ -1976,33 +1971,33 @@
       <c r="M19" s="1">
         <v>98.945816354050606</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="8">
         <v>98.940286378191104</v>
       </c>
-      <c r="O19" s="39"/>
+      <c r="O19" s="33"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="25"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="22"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30"/>
-      <c r="B21" s="7">
+      <c r="A21" s="24"/>
+      <c r="B21" s="6">
         <v>1.6</v>
       </c>
       <c r="C21" s="1">
@@ -2023,13 +2018,13 @@
       <c r="H21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="8">
         <v>98.866232999999994</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="9">
         <v>2.9962000000000001E-4</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="8">
         <v>4.82E-2</v>
       </c>
       <c r="L21" s="1">
@@ -2038,7 +2033,7 @@
       <c r="M21" s="1">
         <v>98.971582625294701</v>
       </c>
-      <c r="N21" s="10">
+      <c r="N21" s="8">
         <v>98.968693643085999</v>
       </c>
       <c r="O21" s="2" t="s">
@@ -2046,8 +2041,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
-      <c r="B22" s="7">
+      <c r="A22" s="24"/>
+      <c r="B22" s="6">
         <v>1.7</v>
       </c>
       <c r="C22" s="1">
@@ -2071,19 +2066,19 @@
       <c r="I22" s="1">
         <v>98.966266000000005</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="15">
         <v>7.5234000000000005E-5</v>
       </c>
       <c r="K22" s="1">
         <v>4.4200000000000003E-2</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="8">
         <v>99.061811284603493</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="8">
         <v>99.061744602502799</v>
       </c>
-      <c r="N22" s="10">
+      <c r="N22" s="8">
         <v>99.061244687099304</v>
       </c>
       <c r="O22" s="2" t="s">
@@ -2091,8 +2086,8 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30"/>
-      <c r="B23" s="7">
+      <c r="A23" s="24"/>
+      <c r="B23" s="6">
         <v>1.8</v>
       </c>
       <c r="C23" s="1">
@@ -2113,13 +2108,13 @@
       <c r="H23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="8">
         <v>98.966265000000007</v>
       </c>
       <c r="J23" s="1">
         <v>1E-3</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="8">
         <v>4.0399999999999998E-2</v>
       </c>
       <c r="L23" s="1">
@@ -2128,7 +2123,7 @@
       <c r="M23" s="1">
         <v>99.055973140102097</v>
       </c>
-      <c r="N23" s="10">
+      <c r="N23" s="8">
         <v>99.055110774851798</v>
       </c>
       <c r="O23" s="2" t="s">
@@ -2136,8 +2131,8 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
-      <c r="B24" s="7">
+      <c r="A24" s="24"/>
+      <c r="B24" s="6">
         <v>1.9</v>
       </c>
       <c r="C24" s="1">
@@ -2150,21 +2145,21 @@
         <v>99.11</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I24" s="10">
+      <c r="I24" s="8">
         <v>99.010731000000007</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="9">
         <v>2.5614000000000002E-4</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="8">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="L24" s="1">
@@ -2173,14 +2168,14 @@
       <c r="M24" s="1">
         <v>99.102820595200001</v>
       </c>
-      <c r="N24" s="10">
+      <c r="N24" s="8">
         <v>99.100256430343094</v>
       </c>
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="30"/>
-      <c r="B25" s="7">
+      <c r="A25" s="24"/>
+      <c r="B25" s="6">
         <v>2</v>
       </c>
       <c r="C25" s="1">
@@ -2193,21 +2188,21 @@
         <v>98.96</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" s="10">
+      <c r="I25" s="8">
         <v>98.843992</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="9">
         <v>9.7678000000000001E-4</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="8">
         <v>4.9299999999999997E-2</v>
       </c>
       <c r="L25" s="1">
@@ -2216,14 +2211,14 @@
       <c r="M25" s="1">
         <v>98.949448401085803</v>
       </c>
-      <c r="N25" s="10">
+      <c r="N25" s="8">
         <v>98.950144585707903</v>
       </c>
       <c r="O25" s="2"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
-      <c r="B26" s="7">
+      <c r="A26" s="24"/>
+      <c r="B26" s="6">
         <v>2.1</v>
       </c>
       <c r="C26" s="1">
@@ -2236,21 +2231,21 @@
         <v>99.01</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I26" s="10">
+      <c r="I26" s="8">
         <v>98.899562000000003</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="9">
         <v>4.2850000000000001E-4</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="8">
         <v>4.8899999999999999E-2</v>
       </c>
       <c r="L26" s="1">
@@ -2259,14 +2254,14 @@
       <c r="M26" s="1">
         <v>98.991518574038494</v>
       </c>
-      <c r="N26" s="10">
+      <c r="N26" s="8">
         <v>98.995367008657198</v>
       </c>
       <c r="O26" s="2"/>
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30"/>
-      <c r="B27" s="7">
+      <c r="A27" s="24"/>
+      <c r="B27" s="6">
         <v>2.2000000000000002</v>
       </c>
       <c r="C27" s="1">
@@ -2279,21 +2274,21 @@
         <v>98.88</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" s="10">
+      <c r="I27" s="8">
         <v>98.755073999999993</v>
       </c>
-      <c r="J27" s="14">
+      <c r="J27" s="9">
         <v>2.2546E-4</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27" s="8">
         <v>5.5199999999999999E-2</v>
       </c>
       <c r="L27" s="1">
@@ -2302,33 +2297,33 @@
       <c r="M27" s="1">
         <v>98.865460635077397</v>
       </c>
-      <c r="N27" s="10">
+      <c r="N27" s="8">
         <v>98.864393927914307</v>
       </c>
       <c r="O27" s="2"/>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30"/>
-      <c r="B28" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="25"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="30"/>
-      <c r="B29" s="7">
+      <c r="A29" s="24"/>
+      <c r="B29" s="6">
         <v>2.2999999999999998</v>
       </c>
       <c r="C29" s="1">
@@ -2341,21 +2336,21 @@
         <v>99.31</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" s="10">
+      <c r="I29" s="8">
         <v>99.233028000000004</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="9">
         <v>4.2316000000000003E-6</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="8">
         <v>4.3200000000000002E-2</v>
       </c>
       <c r="L29" s="1">
@@ -2364,80 +2359,80 @@
       <c r="M29" s="1">
         <v>99.298753186418395</v>
       </c>
-      <c r="N29" s="10">
+      <c r="N29" s="8">
         <v>99.303067584237098</v>
       </c>
       <c r="O29" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="24"/>
+      <c r="B30" s="10">
+        <v>2.4</v>
+      </c>
+      <c r="C30" s="11">
+        <v>40</v>
+      </c>
+      <c r="D30" s="11">
+        <v>16</v>
+      </c>
+      <c r="E30" s="11">
+        <v>99.41</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="30"/>
-      <c r="B30" s="16">
-        <v>2.4</v>
-      </c>
-      <c r="C30" s="17">
-        <v>40</v>
-      </c>
-      <c r="D30" s="17">
-        <v>16</v>
-      </c>
-      <c r="E30" s="17">
-        <v>99.41</v>
-      </c>
-      <c r="F30" s="17" t="s">
+      <c r="G30" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="H30" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H30" s="17" t="s">
+      <c r="I30" s="12">
+        <v>99.344182000000004</v>
+      </c>
+      <c r="J30" s="16">
+        <v>3.2853999999999999E-6</v>
+      </c>
+      <c r="K30" s="12">
+        <v>4.6899999999999997E-2</v>
+      </c>
+      <c r="L30" s="11">
+        <v>99.412401070733793</v>
+      </c>
+      <c r="M30" s="11">
+        <v>99.400879194628004</v>
+      </c>
+      <c r="N30" s="12">
+        <v>99.405751743193505</v>
+      </c>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="I30" s="18">
-        <v>99.344182000000004</v>
-      </c>
-      <c r="J30" s="22">
-        <v>3.2853999999999999E-6</v>
-      </c>
-      <c r="K30" s="18">
-        <v>4.6899999999999997E-2</v>
-      </c>
-      <c r="L30" s="17">
-        <v>99.412401070733793</v>
-      </c>
-      <c r="M30" s="17">
-        <v>99.400879194628004</v>
-      </c>
-      <c r="N30" s="18">
-        <v>99.405751743193505</v>
-      </c>
-      <c r="O30" s="2"/>
-    </row>
-    <row r="31" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="25"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="22"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="27"/>
-      <c r="B32" s="7">
+      <c r="A32" s="35"/>
+      <c r="B32" s="6">
         <v>2.5</v>
       </c>
       <c r="C32" s="1">
@@ -2450,21 +2445,21 @@
         <v>99.52</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I32" s="10">
+      <c r="I32" s="8">
         <v>99.466457000000005</v>
       </c>
       <c r="J32" s="1">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="8">
         <v>2.0899999999999998E-2</v>
       </c>
       <c r="L32" s="1">
@@ -2473,35 +2468,35 @@
       <c r="M32" s="1">
         <v>99.513328949604002</v>
       </c>
-      <c r="N32" s="10">
+      <c r="N32" s="8">
         <v>99.515323065414805</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="27"/>
-      <c r="B33" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="24"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="25"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="22"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27"/>
-      <c r="B34" s="7">
+      <c r="A34" s="35"/>
+      <c r="B34" s="6">
         <v>2.6</v>
       </c>
       <c r="C34" s="1">
@@ -2514,21 +2509,21 @@
         <v>99.59</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I34" s="10">
+      <c r="I34" s="8">
         <v>99.544264999999996</v>
       </c>
       <c r="J34" s="1">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K34" s="8">
         <v>1.21E-2</v>
       </c>
       <c r="L34" s="1">
@@ -2537,16 +2532,16 @@
       <c r="M34" s="1">
         <v>99.585237428860296</v>
       </c>
-      <c r="N34" s="10">
+      <c r="N34" s="8">
         <v>99.587207772325797</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27"/>
-      <c r="B35" s="7">
+      <c r="A35" s="35"/>
+      <c r="B35" s="6">
         <v>2.7</v>
       </c>
       <c r="C35" s="1">
@@ -2559,21 +2554,21 @@
         <v>99.62</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I35" s="10">
+      <c r="I35" s="8">
         <v>99.566501000000002</v>
       </c>
       <c r="J35" s="1">
         <v>2.3900000000000001E-2</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K35" s="8">
         <v>1.18E-2</v>
       </c>
       <c r="L35" s="1">
@@ -2582,57 +2577,57 @@
       <c r="M35" s="1">
         <v>99.612412809604606</v>
       </c>
-      <c r="N35" s="10">
+      <c r="N35" s="8">
         <v>99.6098140371314</v>
       </c>
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
-      <c r="B36" s="40">
+      <c r="A36" s="35"/>
+      <c r="B36" s="17">
         <v>2.8</v>
       </c>
-      <c r="C36" s="41">
+      <c r="C36" s="18">
         <v>30</v>
       </c>
-      <c r="D36" s="41">
+      <c r="D36" s="18">
         <v>16</v>
       </c>
-      <c r="E36" s="41">
+      <c r="E36" s="18">
         <v>99.68</v>
       </c>
-      <c r="F36" s="41" t="s">
+      <c r="F36" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H36" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="G36" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="H36" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="I36" s="42">
+      <c r="I36" s="19">
         <v>99.644305000000003</v>
       </c>
-      <c r="J36" s="41">
+      <c r="J36" s="18">
         <v>2.5399999999999999E-2</v>
       </c>
-      <c r="K36" s="42">
+      <c r="K36" s="19">
         <v>1.11E-2</v>
       </c>
-      <c r="L36" s="41">
+      <c r="L36" s="18">
         <v>99.680366069887796</v>
       </c>
-      <c r="M36" s="41">
+      <c r="M36" s="18">
         <v>99.677054266530206</v>
       </c>
-      <c r="N36" s="42">
+      <c r="N36" s="19">
         <v>99.678523759825197</v>
       </c>
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
-      <c r="B37" s="7">
+      <c r="A37" s="35"/>
+      <c r="B37" s="6">
         <v>2.9</v>
       </c>
       <c r="C37" s="1">
@@ -2645,21 +2640,21 @@
         <v>99.64</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I37" s="10">
+      <c r="I37" s="8">
         <v>99.599846999999997</v>
       </c>
       <c r="J37" s="1">
         <v>2.06E-2</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="8">
         <v>1.24E-2</v>
       </c>
       <c r="L37" s="1">
@@ -2668,14 +2663,14 @@
       <c r="M37" s="1">
         <v>99.644440479456193</v>
       </c>
-      <c r="N37" s="10">
+      <c r="N37" s="8">
         <v>99.642026518247505</v>
       </c>
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="27"/>
-      <c r="B38" s="7">
+      <c r="A38" s="35"/>
+      <c r="B38" s="6">
         <v>3</v>
       </c>
       <c r="C38" s="1">
@@ -2688,21 +2683,21 @@
         <v>99.65</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I38" s="10">
+      <c r="I38" s="8">
         <v>99.610960000000006</v>
       </c>
       <c r="J38" s="1">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="K38" s="10">
+      <c r="K38" s="8">
         <v>1.21E-2</v>
       </c>
       <c r="L38" s="1">
@@ -2711,319 +2706,717 @@
       <c r="M38" s="1">
         <v>99.653051558604702</v>
       </c>
-      <c r="N38" s="10">
+      <c r="N38" s="8">
         <v>99.652617732738705</v>
       </c>
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="27"/>
-      <c r="B39" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="24"/>
-      <c r="O39" s="25"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>27</v>
+      </c>
+      <c r="D39" s="1">
+        <v>16</v>
+      </c>
+      <c r="E39" s="1">
+        <v>99.49</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I39" s="8">
+        <v>99.433108000000004</v>
+      </c>
+      <c r="J39" s="1">
+        <v>2.52E-2</v>
+      </c>
+      <c r="K39" s="8">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="L39" s="1">
+        <v>9.4901073999999994</v>
+      </c>
+      <c r="M39" s="1">
+        <v>99.481993512200006</v>
+      </c>
+      <c r="N39" s="8">
+        <v>99.485719150572194</v>
+      </c>
+      <c r="O39" s="2"/>
     </row>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="27"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="41">
-        <v>35</v>
-      </c>
-      <c r="D40" s="41">
+      <c r="A40" s="35"/>
+      <c r="B40" s="6">
+        <v>3.2</v>
+      </c>
+      <c r="C40" s="1">
+        <v>32</v>
+      </c>
+      <c r="D40" s="1">
         <v>16</v>
       </c>
-      <c r="E40" s="41">
-        <v>99.67</v>
-      </c>
-      <c r="F40" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="G40" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="H40" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="I40" s="42">
-        <v>99.633188000000004</v>
-      </c>
-      <c r="J40" s="41">
-        <v>0.02</v>
-      </c>
-      <c r="K40" s="42">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="L40" s="41">
-        <v>99.670541512184599</v>
-      </c>
-      <c r="M40" s="41">
-        <v>99.663504882977307</v>
-      </c>
-      <c r="N40" s="42">
-        <v>99.666888463563495</v>
+      <c r="E40" s="1">
+        <v>99.63</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I40" s="8">
+        <v>99.588728000000003</v>
+      </c>
+      <c r="J40" s="1">
+        <v>2.35E-2</v>
+      </c>
+      <c r="K40" s="8">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="L40" s="1">
+        <v>99.626991338102798</v>
+      </c>
+      <c r="M40" s="1">
+        <v>99.625491926141095</v>
+      </c>
+      <c r="N40" s="8">
+        <v>99.625942340038506</v>
       </c>
       <c r="O40" s="2"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="27"/>
-      <c r="B41" s="7">
-        <v>3.1</v>
+      <c r="A41" s="35"/>
+      <c r="B41" s="6">
+        <v>3.3</v>
       </c>
       <c r="C41" s="1">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D41" s="1">
         <v>16</v>
       </c>
       <c r="E41" s="1">
-        <v>99.53</v>
+        <v>99.52</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I41" s="10">
-        <v>99.477570999999998</v>
+        <v>145</v>
+      </c>
+      <c r="I41" s="1">
+        <v>99.466451000000006</v>
       </c>
       <c r="J41" s="1">
-        <v>1.67E-2</v>
-      </c>
-      <c r="K41" s="10">
-        <v>1.6899999999999998E-2</v>
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="K41" s="8">
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="L41" s="1">
-        <v>99.531045780225796</v>
+        <v>99.523729200000005</v>
       </c>
       <c r="M41" s="1">
-        <v>99.5246748236044</v>
-      </c>
-      <c r="N41" s="10">
-        <v>99.527555282444695</v>
+        <v>99.509400021827801</v>
+      </c>
+      <c r="N41" s="8">
+        <v>99.516047583982598</v>
       </c>
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="27"/>
-      <c r="B42" s="7">
-        <v>3.2</v>
+      <c r="A42" s="35"/>
+      <c r="B42" s="6">
+        <v>3.4</v>
       </c>
       <c r="C42" s="1">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D42" s="1">
         <v>16</v>
       </c>
       <c r="E42" s="1">
-        <v>99.56</v>
+        <v>99.55</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I42" s="10">
-        <v>99.510914</v>
+        <v>150</v>
+      </c>
+      <c r="I42" s="8">
+        <v>99.499806000000007</v>
       </c>
       <c r="J42" s="1">
-        <v>1.5900000000000001E-2</v>
-      </c>
-      <c r="K42" s="10">
-        <v>1.67E-2</v>
+        <v>2.4E-2</v>
+      </c>
+      <c r="K42" s="8">
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="L42" s="1">
-        <v>99.563259233698503</v>
+        <v>99.548914683005194</v>
       </c>
       <c r="M42" s="1">
-        <v>99.549495507139298</v>
-      </c>
-      <c r="N42" s="10">
-        <v>99.555650691517997</v>
+        <v>99.549282244701004</v>
+      </c>
+      <c r="N42" s="8">
+        <v>99.548576305293594</v>
       </c>
       <c r="O42" s="2"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="27"/>
-      <c r="B43" s="7">
-        <v>3.3</v>
+      <c r="A43" s="35"/>
+      <c r="B43" s="6">
+        <v>3.5</v>
       </c>
       <c r="C43" s="1">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D43" s="1">
         <v>16</v>
       </c>
       <c r="E43" s="1">
-        <v>99.36</v>
+        <v>99.59</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I43" s="10">
-        <v>99.288606000000001</v>
+        <v>156</v>
+      </c>
+      <c r="I43" s="8">
+        <v>99.544263000000001</v>
       </c>
       <c r="J43" s="1">
-        <v>2.1499999999999998E-2</v>
-      </c>
-      <c r="K43" s="10">
-        <v>1.72E-2</v>
+        <v>2.2800000000000001E-2</v>
+      </c>
+      <c r="K43" s="8">
+        <v>1.24E-2</v>
       </c>
       <c r="L43" s="1">
-        <v>99.368582202754993</v>
+        <v>99.594303781420606</v>
       </c>
       <c r="M43" s="1">
-        <v>99.357723776517901</v>
-      </c>
-      <c r="N43" s="10">
-        <v>99.361231044924807</v>
+        <v>99.585284097912194</v>
+      </c>
+      <c r="N43" s="8">
+        <v>99.589516851278006</v>
       </c>
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="27"/>
-      <c r="B44" s="7">
-        <v>3.4</v>
+      <c r="A44" s="35"/>
+      <c r="B44" s="6">
+        <v>3.6</v>
       </c>
       <c r="C44" s="1">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D44" s="1">
         <v>16</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="2"/>
+      <c r="E44" s="1">
+        <v>99.55</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I44" s="8">
+        <v>99.499804999999995</v>
+      </c>
+      <c r="J44" s="1">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="K44" s="8">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="L44" s="1">
+        <v>99.552894248374301</v>
+      </c>
+      <c r="M44" s="1">
+        <v>99.549540142168894</v>
+      </c>
+      <c r="N44" s="8">
+        <v>99.550595714200298</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="27"/>
-      <c r="B45" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="C45" s="1">
+      <c r="A45" s="35"/>
+      <c r="B45" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="22"/>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="35"/>
+      <c r="B46" s="17">
+        <v>3.7</v>
+      </c>
+      <c r="C46" s="18">
+        <v>35</v>
+      </c>
+      <c r="D46" s="18">
+        <v>16</v>
+      </c>
+      <c r="E46" s="18">
+        <v>99.67</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I46" s="19">
+        <v>99.633188000000004</v>
+      </c>
+      <c r="J46" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="K46" s="19">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L46" s="18">
+        <v>99.670541512184599</v>
+      </c>
+      <c r="M46" s="18">
+        <v>99.663504882977307</v>
+      </c>
+      <c r="N46" s="19">
+        <v>99.666888463563495</v>
+      </c>
+      <c r="O46" s="2"/>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="35"/>
+      <c r="B47" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="C47" s="1">
+        <v>45</v>
+      </c>
+      <c r="D47" s="1">
+        <v>16</v>
+      </c>
+      <c r="E47" s="1">
+        <v>99.53</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I47" s="8">
+        <v>99.477570999999998</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1.67E-2</v>
+      </c>
+      <c r="K47" s="8">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="L47" s="1">
+        <v>99.531045780225796</v>
+      </c>
+      <c r="M47" s="1">
+        <v>99.5246748236044</v>
+      </c>
+      <c r="N47" s="8">
+        <v>99.527555282444695</v>
+      </c>
+      <c r="O47" s="2"/>
+    </row>
+    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="35"/>
+      <c r="B48" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="C48" s="1">
+        <v>40</v>
+      </c>
+      <c r="D48" s="1">
+        <v>16</v>
+      </c>
+      <c r="E48" s="1">
+        <v>99.56</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I48" s="8">
+        <v>99.510914</v>
+      </c>
+      <c r="J48" s="1">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="K48" s="8">
+        <v>1.67E-2</v>
+      </c>
+      <c r="L48" s="1">
+        <v>99.563259233698503</v>
+      </c>
+      <c r="M48" s="1">
+        <v>99.549495507139298</v>
+      </c>
+      <c r="N48" s="8">
+        <v>99.555650691517997</v>
+      </c>
+      <c r="O48" s="2"/>
+    </row>
+    <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="35"/>
+      <c r="B49" s="6">
+        <v>4</v>
+      </c>
+      <c r="C49" s="1">
+        <v>30</v>
+      </c>
+      <c r="D49" s="1">
+        <v>16</v>
+      </c>
+      <c r="E49" s="1">
+        <v>99.36</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I49" s="8">
+        <v>99.288606000000001</v>
+      </c>
+      <c r="J49" s="1">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="K49" s="8">
+        <v>1.72E-2</v>
+      </c>
+      <c r="L49" s="1">
+        <v>99.368582202754993</v>
+      </c>
+      <c r="M49" s="1">
+        <v>99.357723776517901</v>
+      </c>
+      <c r="N49" s="8">
+        <v>99.361231044924807</v>
+      </c>
+      <c r="O49" s="2"/>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="35"/>
+      <c r="B50" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="22"/>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="35"/>
+      <c r="B51" s="6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C51" s="1">
         <v>50</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D51" s="1">
         <v>32</v>
       </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="2"/>
-    </row>
-    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="2"/>
-    </row>
-    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="27"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="2"/>
-    </row>
-    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="27"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="2"/>
-    </row>
-    <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="28"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="13"/>
-    </row>
-    <row r="50" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E51" s="1">
+        <v>99.6</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I51" s="8">
+        <v>99.555379000000002</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="K51" s="8">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="L51" s="1">
+        <v>99.601663766054202</v>
+      </c>
+      <c r="M51" s="1">
+        <v>99.593148103666607</v>
+      </c>
+      <c r="N51" s="8">
+        <v>99.597047935612594</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="35"/>
+      <c r="B52" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>30</v>
+      </c>
+      <c r="D52" s="1">
+        <v>32</v>
+      </c>
+      <c r="E52" s="1">
+        <v>99.59</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I52" s="8">
+        <v>99.544269</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="K52" s="8">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="L52" s="1">
+        <v>99.587862868490603</v>
+      </c>
+      <c r="M52" s="1">
+        <v>99.59026190873</v>
+      </c>
+      <c r="N52" s="8">
+        <v>99.588836662708701</v>
+      </c>
+      <c r="O52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="35"/>
+      <c r="B53" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="C53" s="1">
+        <v>40</v>
+      </c>
+      <c r="D53" s="1">
+        <v>32</v>
+      </c>
+      <c r="E53" s="1">
+        <v>99.61</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I53" s="8">
+        <v>99.566496000000001</v>
+      </c>
+      <c r="J53" s="1">
+        <v>1.66E-2</v>
+      </c>
+      <c r="K53" s="8">
+        <v>1.61E-2</v>
+      </c>
+      <c r="L53" s="1">
+        <v>99.611709734635895</v>
+      </c>
+      <c r="M53" s="1">
+        <v>99.607843319654606</v>
+      </c>
+      <c r="N53" s="8">
+        <v>99.609292494218494</v>
+      </c>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="35"/>
+      <c r="B54" s="6">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C54" s="1">
+        <v>38</v>
+      </c>
+      <c r="D54" s="1">
+        <v>32</v>
+      </c>
+      <c r="E54" s="1">
+        <v>99.53</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="J54" s="1">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="K54" s="8">
+        <v>1.44E-2</v>
+      </c>
+      <c r="L54" s="1">
+        <v>99.530397336899398</v>
+      </c>
+      <c r="M54" s="1">
+        <v>99.522652095165498</v>
+      </c>
+      <c r="N54" s="8">
+        <v>99.526008155265998</v>
+      </c>
+      <c r="O54" s="2"/>
+    </row>
+    <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="35"/>
+      <c r="B55" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="C55" s="1">
+        <v>38</v>
+      </c>
+      <c r="D55" s="1">
+        <v>32</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="2"/>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="35"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="2"/>
+    </row>
+    <row r="57" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="B57:O57"/>
     <mergeCell ref="B33:O33"/>
-    <mergeCell ref="A31:A49"/>
     <mergeCell ref="B28:O28"/>
     <mergeCell ref="B31:O31"/>
     <mergeCell ref="A2:A30"/>
@@ -3033,7 +3426,9 @@
     <mergeCell ref="E11:O11"/>
     <mergeCell ref="B20:O20"/>
     <mergeCell ref="O17:O19"/>
-    <mergeCell ref="B39:O39"/>
+    <mergeCell ref="B45:O45"/>
+    <mergeCell ref="B50:O50"/>
+    <mergeCell ref="A31:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed excel file with all versions and their performance. Structured the code better and added extra comments. Renamed some files. Changed save directory for all notebook outputs. Added extra trained models in the /trained_models/ directory.
</commit_message>
<xml_diff>
--- a/Model Performance.xlsx
+++ b/Model Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Academia\Kings_College_London\Semester_2\Deep_Learning_&amp;_Neural_Networks\Coursework_I\MNIST_deeplearning_recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD457CF2-C990-491F-A0A4-DFDA5A6D584E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2781EB-E47E-42E7-A4F7-6C14F14565C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24255" yWindow="1395" windowWidth="27975" windowHeight="29970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="189">
   <si>
     <t>version</t>
   </si>
@@ -517,13 +517,88 @@
   </si>
   <si>
     <t> 99.477571</t>
+  </si>
+  <si>
+    <t>99.80, 99.91, 99.81, 99.41, 99.29, 99.89, 99.58, 99.42, 99.79, 99.60</t>
+  </si>
+  <si>
+    <t>99.80, 99.74, 99.71, 100.00, 99.39, 99.22, 99.90, 99.71, 99.79, 99.21</t>
+  </si>
+  <si>
+    <t>99.80, 99.82, 99.76, 99.70, 99.34, 99.55, 99.74, 99.56, 99.79, 99.40</t>
+  </si>
+  <si>
+    <t>99.69, 99.65, 99.71, 99.31, 99.29, 99.33, 100.00, 99.81, 99.90, 99.70</t>
+  </si>
+  <si>
+    <t>100.00, 99.91, 99.81, 99.60, 99.80, 99.78, 99.27, 99.71, 99.28, 99.21</t>
+  </si>
+  <si>
+    <t>99.85, 99.78, 99.76, 99.46, 99.54, 99.55, 99.63, 99.76, 99.59, 99.45</t>
+  </si>
+  <si>
+    <t>64 neurons dense layer</t>
+  </si>
+  <si>
+    <t>256 neurons dense layer</t>
+  </si>
+  <si>
+    <t>99.80, 99.91, 99.71, 99.31, 99.59, 99.77, 99.37, 99.03, 99.69, 99.70</t>
+  </si>
+  <si>
+    <t>99.80, 99.56, 99.52, 100.00, 99.49, 99.22, 99.48, 99.81, 99.79, 99.21</t>
+  </si>
+  <si>
+    <t>99.80, 99.74, 99.61, 99.65, 99.54, 99.49, 99.43, 99.42, 99.74, 99.45</t>
+  </si>
+  <si>
+    <t>99.69, 99.56, 99.52, 99.51, 99.39, 99.66, 99.90, 99.32, 99.90, 99.50</t>
+  </si>
+  <si>
+    <t>99.69, 99.82, 99.71, 99.90, 99.39, 99.55, 99.48, 99.42, 99.49, 99.41</t>
+  </si>
+  <si>
+    <t>99.69, 99.69, 99.61, 99.70, 99.39, 99.61, 99.69, 99.37, 99.69, 99.45</t>
+  </si>
+  <si>
+    <t>ENSEMBLE</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>99.90, 99.65, 99.81, 99.80, 99.80, 99.78, 99.69, 99.90, 99.79, 99.80</t>
+  </si>
+  <si>
+    <t>99.90, 99.91, 100.00, 99.90, 99.80, 99.78, 99.58, 99.71, 99.59, 99.70</t>
+  </si>
+  <si>
+    <t>99.90, 99.78, 99.90, 99.85, 99.80, 99.78, 99.63, 99.81, 99.69, 99.75</t>
+  </si>
+  <si>
+    <t>2 CNNs prediction</t>
+  </si>
+  <si>
+    <t>99.90, 99.74, 99.71, 99.70, 99.59, 99.66, 99.90, 99.61, 99.79, 99.70</t>
+  </si>
+  <si>
+    <t>100.00, 99.91, 99.81, 99.90, 99.59, 99.78, 99.48, 99.81, 99.49, 99.50</t>
+  </si>
+  <si>
+    <t>99.95, 99.82, 99.76, 99.80, 99.59, 99.72, 99.69, 99.71, 99.64, 99.60</t>
+  </si>
+  <si>
+    <t>3 CNNs prediction</t>
+  </si>
+  <si>
+    <t>4 CNNs prediction (same performance as v4.9)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +618,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -598,7 +681,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -862,11 +945,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -965,11 +1085,17 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1251,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E61" sqref="D61:E61"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O66" sqref="O66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2410,7 +2536,7 @@
       <c r="O30" s="2"/>
     </row>
     <row r="31" spans="1:15" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="23" t="s">
         <v>152</v>
       </c>
       <c r="B31" s="20" t="s">
@@ -2431,7 +2557,7 @@
       <c r="O31" s="22"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="6">
         <v>2.5</v>
       </c>
@@ -2476,7 +2602,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="20" t="s">
         <v>97</v>
       </c>
@@ -2495,7 +2621,7 @@
       <c r="O33" s="22"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="35"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="6">
         <v>2.6</v>
       </c>
@@ -2540,7 +2666,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="35"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="6">
         <v>2.7</v>
       </c>
@@ -2583,7 +2709,7 @@
       <c r="O35" s="2"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="35"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="17">
         <v>2.8</v>
       </c>
@@ -2626,7 +2752,7 @@
       <c r="O36" s="2"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="35"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="6">
         <v>2.9</v>
       </c>
@@ -2669,7 +2795,7 @@
       <c r="O37" s="2"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="35"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="6">
         <v>3</v>
       </c>
@@ -2712,7 +2838,7 @@
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="35"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="6">
         <v>3.1</v>
       </c>
@@ -2755,7 +2881,7 @@
       <c r="O39" s="2"/>
     </row>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="35"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="6">
         <v>3.2</v>
       </c>
@@ -2798,7 +2924,7 @@
       <c r="O40" s="2"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="35"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="6">
         <v>3.3</v>
       </c>
@@ -2841,7 +2967,7 @@
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="35"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="6">
         <v>3.4</v>
       </c>
@@ -2884,7 +3010,7 @@
       <c r="O42" s="2"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="35"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="6">
         <v>3.5</v>
       </c>
@@ -2927,7 +3053,7 @@
       <c r="O43" s="2"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="35"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="6">
         <v>3.6</v>
       </c>
@@ -2972,7 +3098,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="35"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="20" t="s">
         <v>111</v>
       </c>
@@ -2991,7 +3117,7 @@
       <c r="O45" s="22"/>
     </row>
     <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="35"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="17">
         <v>3.7</v>
       </c>
@@ -3034,7 +3160,7 @@
       <c r="O46" s="2"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="35"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="6">
         <v>3.8</v>
       </c>
@@ -3077,7 +3203,7 @@
       <c r="O47" s="2"/>
     </row>
     <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="35"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="6">
         <v>3.9</v>
       </c>
@@ -3120,7 +3246,7 @@
       <c r="O48" s="2"/>
     </row>
     <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="35"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="6">
         <v>4</v>
       </c>
@@ -3163,7 +3289,7 @@
       <c r="O49" s="2"/>
     </row>
     <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="35"/>
+      <c r="A50" s="24"/>
       <c r="B50" s="20" t="s">
         <v>127</v>
       </c>
@@ -3182,7 +3308,7 @@
       <c r="O50" s="22"/>
     </row>
     <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="35"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="6">
         <v>4.0999999999999996</v>
       </c>
@@ -3227,7 +3353,7 @@
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="35"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="6">
         <v>4.2</v>
       </c>
@@ -3270,7 +3396,7 @@
       <c r="O52" s="2"/>
     </row>
     <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="35"/>
+      <c r="A53" s="24"/>
       <c r="B53" s="6">
         <v>4.3</v>
       </c>
@@ -3313,7 +3439,7 @@
       <c r="O53" s="2"/>
     </row>
     <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="35"/>
+      <c r="A54" s="24"/>
       <c r="B54" s="6">
         <v>4.4000000000000004</v>
       </c>
@@ -3356,66 +3482,341 @@
       <c r="O54" s="2"/>
     </row>
     <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="35"/>
+      <c r="A55" s="24"/>
       <c r="B55" s="6">
         <v>4.5</v>
       </c>
       <c r="C55" s="1">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D55" s="1">
         <v>32</v>
       </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="2"/>
+      <c r="E55" s="1">
+        <v>99.65</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I55" s="34">
+        <v>99.610957999999997</v>
+      </c>
+      <c r="J55" s="8">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="K55" s="8">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="L55" s="1">
+        <v>99.649660578358606</v>
+      </c>
+      <c r="M55" s="1">
+        <v>99.6450736227319</v>
+      </c>
+      <c r="N55" s="8">
+        <v>99.647068885596894</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="35"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="8"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C56" s="1">
+        <v>100</v>
+      </c>
+      <c r="D56" s="1">
+        <v>32</v>
+      </c>
+      <c r="E56" s="1">
+        <v>99.64</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I56" s="8">
+        <v>99.599843000000007</v>
+      </c>
+      <c r="J56" s="1">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="K56" s="8">
+        <v>1.26E-2</v>
+      </c>
+      <c r="L56" s="1">
+        <v>99.638616965841194</v>
+      </c>
+      <c r="M56" s="1">
+        <v>99.636010720245693</v>
+      </c>
+      <c r="N56" s="8">
+        <v>99.636842165821903</v>
+      </c>
       <c r="O56" s="2"/>
     </row>
     <row r="57" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="20" t="s">
+      <c r="A57" s="24"/>
+      <c r="B57" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="C57" s="1">
+        <v>98</v>
+      </c>
+      <c r="D57" s="1">
+        <v>32</v>
+      </c>
+      <c r="E57" s="1">
+        <v>99.59</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I57" s="34">
+        <v>99.544265999999993</v>
+      </c>
+      <c r="J57" s="8">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="K57" s="8">
+        <v>1.46E-2</v>
+      </c>
+      <c r="L57" s="1">
+        <v>99.589731386896105</v>
+      </c>
+      <c r="M57" s="1">
+        <v>99.586229984799701</v>
+      </c>
+      <c r="N57" s="8">
+        <v>99.587524121754399</v>
+      </c>
+      <c r="O57" s="2"/>
+    </row>
+    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="24"/>
+      <c r="B58" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="C58" s="1">
+        <v>100</v>
+      </c>
+      <c r="D58" s="1">
+        <v>16</v>
+      </c>
+      <c r="E58" s="1">
+        <v>99.59</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I58" s="8">
+        <v>99.544262000000003</v>
+      </c>
+      <c r="J58" s="1">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="K58" s="8">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="L58" s="1">
+        <v>99.594593785745204</v>
+      </c>
+      <c r="M58" s="1">
+        <v>99.585495662055706</v>
+      </c>
+      <c r="N58" s="8">
+        <v>99.589885318223807</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="B59" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="21"/>
-      <c r="M57" s="21"/>
-      <c r="N57" s="21"/>
-      <c r="O57" s="22"/>
-    </row>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
+      <c r="M59" s="21"/>
+      <c r="N59" s="21"/>
+      <c r="O59" s="22"/>
+    </row>
+    <row r="60" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="36"/>
+      <c r="B60" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E60" s="1">
+        <v>99.79</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I60" s="8">
+        <v>99.766574000000006</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="L60" s="1">
+        <v>99.791221703997394</v>
+      </c>
+      <c r="M60" s="1">
+        <v>99.786559529185197</v>
+      </c>
+      <c r="N60" s="8">
+        <v>99.788836266537004</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="36"/>
+      <c r="B61" s="6">
+        <v>5</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E61" s="1">
+        <v>99.79</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I61" s="8">
+        <v>99.766574000000006</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="L61" s="1">
+        <v>99.791221703997394</v>
+      </c>
+      <c r="M61" s="1">
+        <v>99.786559529185197</v>
+      </c>
+      <c r="N61" s="8">
+        <v>99.788836266537004</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="37"/>
+      <c r="B62" s="6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E62" s="1">
+        <v>99.73</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I62" s="8">
+        <v>99.699882000000002</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K62" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="L62" s="1">
+        <v>99.730701464405897</v>
+      </c>
+      <c r="M62" s="1">
+        <v>99.726217834174804</v>
+      </c>
+      <c r="N62" s="8">
+        <v>99.728347527372804</v>
+      </c>
+      <c r="O62" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B57:O57"/>
+  <mergeCells count="15">
+    <mergeCell ref="B59:O59"/>
     <mergeCell ref="B33:O33"/>
     <mergeCell ref="B28:O28"/>
     <mergeCell ref="B31:O31"/>
@@ -3428,7 +3829,8 @@
     <mergeCell ref="O17:O19"/>
     <mergeCell ref="B45:O45"/>
     <mergeCell ref="B50:O50"/>
-    <mergeCell ref="A31:A56"/>
+    <mergeCell ref="A31:A58"/>
+    <mergeCell ref="A59:A62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>